<commit_message>
Modificacion desde carpeta externa
</commit_message>
<xml_diff>
--- a/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
+++ b/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc71912cadc963b0/Documentos/HALCO/PRUEBAS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc71912cadc963b0/Documentos/HALCO/folder/prueba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_AD4D2F04E46CFB4ACB3E20EF4515D9B4683EDF22" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AF2CA5F-F7C1-4174-9F3E-9B6CA90ED596}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_AD4D2F04E46CFB4ACB3E20EF4515D9B4683EDF22" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{309245B5-E953-4E8D-AEE0-593CCA505419}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,12 +52,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,33 +361,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>